<commit_message>
Updated main.py, data source and README.md
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiothon/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiothon/Desktop/Code/Smoking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA6B43DB-1F9B-9D42-B69E-4C86501E3BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9B0A65-B740-F141-AFE1-141C66D51CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17100" activeTab="1" xr2:uid="{CF439FE3-60EE-234D-B1D1-D0B917F16B64}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17100" xr2:uid="{CF439FE3-60EE-234D-B1D1-D0B917F16B64}"/>
   </bookViews>
   <sheets>
-    <sheet name="Demographic" sheetId="1" r:id="rId1"/>
-    <sheet name="Odds Ratio" sheetId="2" r:id="rId2"/>
+    <sheet name="Odds Ratio" sheetId="2" r:id="rId1"/>
+    <sheet name="Demographic" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Odds Ratio'!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>Smoking Category</t>
   </si>
@@ -69,65 +72,191 @@
     <t>Smoking Quantity</t>
   </si>
   <si>
-    <t>Overall OR (95% CI)</t>
-  </si>
-  <si>
-    <t>Men OR (95% CI)</t>
-  </si>
-  <si>
-    <t>Women OR (95% CI)</t>
-  </si>
-  <si>
-    <t>5.79 (5.26-6.38)</t>
-  </si>
-  <si>
-    <t>5.61 (4.94-6.38)</t>
-  </si>
-  <si>
-    <t>5.75 (4.95-6.68)</t>
-  </si>
-  <si>
-    <t>9.37 (8.63-10.17)</t>
-  </si>
-  <si>
-    <t>8.24 (7.36-9.24)</t>
-  </si>
-  <si>
-    <t>10.78 (9.57-12.15)</t>
-  </si>
-  <si>
-    <t>15.13 (14.00-16.30)</t>
-  </si>
-  <si>
-    <t>12.81 (11.52-14.24)</t>
-  </si>
-  <si>
-    <t>19.10 (16.98-21.49)</t>
-  </si>
-  <si>
-    <t>3.61 (3.34-3.91)</t>
-  </si>
-  <si>
-    <t>3.60 (3.23-3.99)</t>
-  </si>
-  <si>
-    <t>3.32 (2.93-3.75)</t>
-  </si>
-  <si>
-    <t>1.29 (1.15-1.45)</t>
-  </si>
-  <si>
-    <t>1.21 (1.04-1.41)</t>
-  </si>
-  <si>
-    <t>1.34 (1.13-1.60)</t>
+    <t>Demographic</t>
+  </si>
+  <si>
+    <t>Case Subjects (N = 12,062)</t>
+  </si>
+  <si>
+    <t>Control Subjects (N = 47,980)</t>
+  </si>
+  <si>
+    <t>Total (%)</t>
+  </si>
+  <si>
+    <t>Case Subjects (Men)</t>
+  </si>
+  <si>
+    <t>Control Subjects (Men)</t>
+  </si>
+  <si>
+    <t>Total (Men %)</t>
+  </si>
+  <si>
+    <t>Case Subjects (Women)</t>
+  </si>
+  <si>
+    <t>Control Subjects (Women)</t>
+  </si>
+  <si>
+    <t>Total (Women %)</t>
+  </si>
+  <si>
+    <t>Median Length of Data Collection (years)</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>1,213 (10.1)</t>
+  </si>
+  <si>
+    <t>17,976 (37.5)</t>
+  </si>
+  <si>
+    <t>577 (8.1)</t>
+  </si>
+  <si>
+    <t>8,655 (30.5)</t>
+  </si>
+  <si>
+    <t>636 (12.9)</t>
+  </si>
+  <si>
+    <t>9,321 (47.5)</t>
+  </si>
+  <si>
+    <t>Trivial/Light</t>
+  </si>
+  <si>
+    <t>1,030 (8.5)</t>
+  </si>
+  <si>
+    <t>3,113 (6.5)</t>
+  </si>
+  <si>
+    <t>640 (9.0)</t>
+  </si>
+  <si>
+    <t>1,978 (7.0)</t>
+  </si>
+  <si>
+    <t>390 (7.9)</t>
+  </si>
+  <si>
+    <t>1,135 (5.8)</t>
+  </si>
+  <si>
+    <t>2,465 (20.4)</t>
+  </si>
+  <si>
+    <t>4,859 (10.1)</t>
+  </si>
+  <si>
+    <t>1,303 (18.2)</t>
+  </si>
+  <si>
+    <t>2,904 (10.2)</t>
+  </si>
+  <si>
+    <t>1,162 (23.6)</t>
+  </si>
+  <si>
+    <t>1,955 (10.0)</t>
+  </si>
+  <si>
+    <t>4,547 (37.7)</t>
+  </si>
+  <si>
+    <t>6,051 (12.6)</t>
+  </si>
+  <si>
+    <t>2,712 (38.0)</t>
+  </si>
+  <si>
+    <t>4,102 (14.5)</t>
+  </si>
+  <si>
+    <t>1,835 (37.3)</t>
+  </si>
+  <si>
+    <t>1,949 (9.9)</t>
+  </si>
+  <si>
+    <t>Smoker but Unknown Quantity</t>
+  </si>
+  <si>
+    <t>2,285 (18.9)</t>
+  </si>
+  <si>
+    <t>10,732 (22.4)</t>
+  </si>
+  <si>
+    <t>1,607 (22.5)</t>
+  </si>
+  <si>
+    <t>7,364 (26.0)</t>
+  </si>
+  <si>
+    <t>678 (13.8)</t>
+  </si>
+  <si>
+    <t>3,368 (17.1)</t>
+  </si>
+  <si>
+    <t>Missing Smoking Status</t>
+  </si>
+  <si>
+    <t>522 (4.3)</t>
+  </si>
+  <si>
+    <t>5,249 (10.9)</t>
+  </si>
+  <si>
+    <t>304 (4.3)</t>
+  </si>
+  <si>
+    <t>3,335 (11.8)</t>
+  </si>
+  <si>
+    <t>218 (4.4)</t>
+  </si>
+  <si>
+    <t>1,914 (9.7)</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>men</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>or_lower</t>
+  </si>
+  <si>
+    <t>or_upper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +277,13 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -171,12 +307,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,95 +657,318 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A488C0B3-771B-314C-9B9D-BB0181F5181B}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B055C-AA64-B24D-9244-AF780370AC38}">
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5.26</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6.38</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5.61</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6.38</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4.95</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6.68</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="C4" s="2">
-        <v>10.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="3">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8.24</v>
+      </c>
+      <c r="E9" s="3">
+        <v>7.36</v>
+      </c>
+      <c r="F9" s="3">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="3">
+        <v>10.78</v>
+      </c>
+      <c r="E10" s="3">
+        <v>9.57</v>
+      </c>
+      <c r="F10" s="3">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="C5" s="2">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="C6" s="2">
-        <v>22.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>4.3</v>
-      </c>
-      <c r="C7" s="2">
-        <v>10.9</v>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="3">
+        <v>15.13</v>
+      </c>
+      <c r="E11" s="3">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="3">
+        <v>12.81</v>
+      </c>
+      <c r="E12" s="3">
+        <v>11.52</v>
+      </c>
+      <c r="F12" s="3">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E13" s="3">
+        <v>16.98</v>
+      </c>
+      <c r="F13" s="3">
+        <v>21.49</v>
       </c>
     </row>
   </sheetData>
@@ -608,117 +977,363 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B055C-AA64-B24D-9244-AF780370AC38}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A488C0B3-771B-314C-9B9D-BB0181F5181B}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>10.1</v>
       </c>
       <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="C5" s="3">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="C6" s="3">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9.5399999999999991</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.56</v>
+      </c>
+      <c r="D10" s="4">
+        <v>9.56</v>
+      </c>
+      <c r="E10" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="F10" s="4">
+        <v>9.64</v>
+      </c>
+      <c r="G10" s="4">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="H10" s="4">
+        <v>9.48</v>
+      </c>
+      <c r="I10" s="4">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="J10" s="4">
+        <v>9.4700000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4">
+        <v>32</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="G12" s="4">
         <v>26</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="H12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="J12" s="4">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4">
+        <v>6.9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="4">
+        <v>7.4</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="4">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="4">
+        <v>11.9</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="4">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4">
+        <v>17.7</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="4">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4">
+        <v>21.7</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="4">
+        <v>25.3</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="4">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="4">
+        <v>9.6</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="4">
+        <v>8.6999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data.xlsx, main.py and README
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiothon/Desktop/Code/Smoking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9B0A65-B740-F141-AFE1-141C66D51CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E73414E-318F-6B4D-9884-FEEF3AB6B43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17100" xr2:uid="{CF439FE3-60EE-234D-B1D1-D0B917F16B64}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17100" activeTab="1" xr2:uid="{CF439FE3-60EE-234D-B1D1-D0B917F16B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Odds Ratio" sheetId="2" r:id="rId1"/>
-    <sheet name="Demographic" sheetId="1" r:id="rId2"/>
+    <sheet name="Synthetic data" sheetId="3" r:id="rId2"/>
+    <sheet name="Demographic" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Odds Ratio'!$A$1:$F$1</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="70">
   <si>
     <t>Smoking Category</t>
   </si>
@@ -660,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B055C-AA64-B24D-9244-AF780370AC38}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="118" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,11 +978,3710 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DC3EDA-C558-7A41-8B53-C3CD70AEBAC5}">
+  <dimension ref="A1:F184"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5.9314400393938396</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F5" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="4">
+        <v>6.2421400953281552</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F6" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5.7373843173326167</v>
+      </c>
+      <c r="E7" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="4">
+        <v>6.2827731473713877</v>
+      </c>
+      <c r="E8" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6.1592675402245849</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F9" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5.7925638073673529</v>
+      </c>
+      <c r="E10" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F10" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5.5879328782194468</v>
+      </c>
+      <c r="E11" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F11" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="4">
+        <v>6.3119452885534004</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F12" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5.3648644771185277</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F13" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5.559178093021977</v>
+      </c>
+      <c r="E14" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F14" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5.7261872012244064</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F15" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5.7673114791828226</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F16" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5.6212462603560391</v>
+      </c>
+      <c r="E17" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F17" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5.9438893726487869</v>
+      </c>
+      <c r="E18" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F18" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5.6531796918256614</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F19" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="4">
+        <v>6.3710533633578956</v>
+      </c>
+      <c r="E20" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F20" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="4">
+        <v>2</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5.8857351928358561</v>
+      </c>
+      <c r="E21" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F21" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6.1941973793171297</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F22" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5.8403073274648811</v>
+      </c>
+      <c r="E23" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F23" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="4">
+        <v>2</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5.6628488237785506</v>
+      </c>
+      <c r="E24" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="F24" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="4">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5.0728316166452494</v>
+      </c>
+      <c r="E25" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F25" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="4">
+        <v>5.4973877783701974</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F26" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="4">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="4">
+        <v>5.3868892890284936</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F27" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5.9200617264578996</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F28" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="4">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="4">
+        <v>5.1549274165855872</v>
+      </c>
+      <c r="E29" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F29" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="4">
+        <v>2</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="4">
+        <v>5.3881838557832218</v>
+      </c>
+      <c r="E30" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F30" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="4">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="4">
+        <v>5.6858577743988281</v>
+      </c>
+      <c r="E31" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F31" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="4">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5.2079465707325516</v>
+      </c>
+      <c r="E32" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F32" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.2837838464846367</v>
+      </c>
+      <c r="E33" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F33" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="4">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="4">
+        <v>6.081607425998822</v>
+      </c>
+      <c r="E34" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F34" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="4">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="4">
+        <v>5.5669229461377627</v>
+      </c>
+      <c r="E35" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F35" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="4">
+        <v>5.3147035557684319</v>
+      </c>
+      <c r="E36" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F36" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="4">
+        <v>2</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="4">
+        <v>5.9236925370544444</v>
+      </c>
+      <c r="E37" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F37" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="4">
+        <v>5.659365877670937</v>
+      </c>
+      <c r="E38" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F38" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="4">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="4">
+        <v>6.0561043877420504</v>
+      </c>
+      <c r="E39" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F39" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="4">
+        <v>2</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="4">
+        <v>5.0092077287925862</v>
+      </c>
+      <c r="E40" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F40" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="4">
+        <v>5.6124045025191114</v>
+      </c>
+      <c r="E41" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F41" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="4">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="4">
+        <v>5.0260528186799576</v>
+      </c>
+      <c r="E42" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F42" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="4">
+        <v>2</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="4">
+        <v>5.5706946087907649</v>
+      </c>
+      <c r="E43" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F43" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="4">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="4">
+        <v>6.3396387595838597</v>
+      </c>
+      <c r="E44" s="4">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F44" s="4">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4">
+        <v>2</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="4">
+        <v>6.5392119359374892</v>
+      </c>
+      <c r="E45" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F45" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="4">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="4">
+        <v>5.8064522621786399</v>
+      </c>
+      <c r="E46" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F46" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="4">
+        <v>2</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="4">
+        <v>6.3673924071594534</v>
+      </c>
+      <c r="E47" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F47" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="4">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="4">
+        <v>5.3165247766134076</v>
+      </c>
+      <c r="E48" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F48" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="4">
+        <v>5.6982562368331768</v>
+      </c>
+      <c r="E49" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F49" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="4">
+        <v>2</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="4">
+        <v>6.49520547079005</v>
+      </c>
+      <c r="E50" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F50" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="4">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="4">
+        <v>5.8667813806266276</v>
+      </c>
+      <c r="E51" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F51" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="4">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="4">
+        <v>6.3746587662060046</v>
+      </c>
+      <c r="E52" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F52" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="4">
+        <v>2</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="4">
+        <v>5.7719719071671651</v>
+      </c>
+      <c r="E53" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F53" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="4">
+        <v>2</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="4">
+        <v>6.1510380700340992</v>
+      </c>
+      <c r="E54" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F54" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="4">
+        <v>6.6525741397519784</v>
+      </c>
+      <c r="E55" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F55" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="4">
+        <v>2</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" s="4">
+        <v>5.5453126132180106</v>
+      </c>
+      <c r="E56" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F56" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="4">
+        <v>2</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="4">
+        <v>5.4517523139992186</v>
+      </c>
+      <c r="E57" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F57" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="4">
+        <v>2</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="4">
+        <v>6.4215426611032003</v>
+      </c>
+      <c r="E58" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F58" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="4">
+        <v>2</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="4">
+        <v>6.5510653190658958</v>
+      </c>
+      <c r="E59" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F59" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="4">
+        <v>2</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="4">
+        <v>5.5618471218099126</v>
+      </c>
+      <c r="E60" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F60" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="4">
+        <v>2</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="4">
+        <v>5.7667928682114837</v>
+      </c>
+      <c r="E61" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F61" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="4">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="4">
+        <v>5.4290095068229336</v>
+      </c>
+      <c r="E62" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F62" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="4">
+        <v>2</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="4">
+        <v>5.0367941180930353</v>
+      </c>
+      <c r="E63" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F63" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="4">
+        <v>2</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="4">
+        <v>5.0411161961979394</v>
+      </c>
+      <c r="E64" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="F64" s="4">
+        <v>6.68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="4">
+        <v>3</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" s="4">
+        <v>9.9801328311193895</v>
+      </c>
+      <c r="E65" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F65" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="4">
+        <v>3</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="4">
+        <v>9.3602763744015594</v>
+      </c>
+      <c r="E66" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F66" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="4">
+        <v>3</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" s="4">
+        <v>9.601830498674536</v>
+      </c>
+      <c r="E67" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F67" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="4">
+        <v>3</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" s="4">
+        <v>8.6334835150223466</v>
+      </c>
+      <c r="E68" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F68" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="4">
+        <v>3</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="4">
+        <v>9.9050700807654515</v>
+      </c>
+      <c r="E69" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F69" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="4">
+        <v>3</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="4">
+        <v>8.6438179902196932</v>
+      </c>
+      <c r="E70" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F70" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="4">
+        <v>3</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="4">
+        <v>9.7310682673442486</v>
+      </c>
+      <c r="E71" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F71" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="4">
+        <v>3</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="4">
+        <v>9.4633147768057153</v>
+      </c>
+      <c r="E72" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F72" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="4">
+        <v>3</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" s="4">
+        <v>9.701165700864399</v>
+      </c>
+      <c r="E73" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F73" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="4">
+        <v>3</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" s="4">
+        <v>9.1756447826749703</v>
+      </c>
+      <c r="E74" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F74" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="4">
+        <v>3</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="4">
+        <v>9.6728719695601679</v>
+      </c>
+      <c r="E75" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F75" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="4">
+        <v>3</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="4">
+        <v>9.3939353313307876</v>
+      </c>
+      <c r="E76" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F76" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="4">
+        <v>3</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="4">
+        <v>9.7838530023014645</v>
+      </c>
+      <c r="E77" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F77" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="4">
+        <v>3</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D78" s="4">
+        <v>9.8608629059477675</v>
+      </c>
+      <c r="E78" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F78" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="4">
+        <v>3</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D79" s="4">
+        <v>9.8384029701855642</v>
+      </c>
+      <c r="E79" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F79" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="4">
+        <v>3</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D80" s="4">
+        <v>9.710663492940963</v>
+      </c>
+      <c r="E80" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F80" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="4">
+        <v>3</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D81" s="4">
+        <v>9.0132956985045087</v>
+      </c>
+      <c r="E81" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F81" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="4">
+        <v>3</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" s="4">
+        <v>9.7217401143621238</v>
+      </c>
+      <c r="E82" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F82" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="4">
+        <v>3</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="4">
+        <v>9.8291949257075846</v>
+      </c>
+      <c r="E83" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F83" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="4">
+        <v>3</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" s="4">
+        <v>8.9015002769975258</v>
+      </c>
+      <c r="E84" s="4">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F84" s="4">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="4">
+        <v>3</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D85" s="4">
+        <v>8.627971179595022</v>
+      </c>
+      <c r="E85" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F85" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="4">
+        <v>3</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D86" s="4">
+        <v>8.3058053935794725</v>
+      </c>
+      <c r="E86" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F86" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="4">
+        <v>3</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D87" s="4">
+        <v>7.815944703414945</v>
+      </c>
+      <c r="E87" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F87" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="4">
+        <v>3</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D88" s="4">
+        <v>8.0853165086545733</v>
+      </c>
+      <c r="E88" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F88" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="4">
+        <v>3</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D89" s="4">
+        <v>8.9881772814795422</v>
+      </c>
+      <c r="E89" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F89" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="4">
+        <v>3</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D90" s="4">
+        <v>8.7743576275243615</v>
+      </c>
+      <c r="E90" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F90" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="4">
+        <v>3</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D91" s="4">
+        <v>8.8262420120228935</v>
+      </c>
+      <c r="E91" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F91" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="4">
+        <v>3</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D92" s="4">
+        <v>7.8327852909058251</v>
+      </c>
+      <c r="E92" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F92" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="4">
+        <v>3</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D93" s="4">
+        <v>8.5131952910379241</v>
+      </c>
+      <c r="E93" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F93" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="4">
+        <v>3</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D94" s="4">
+        <v>7.5201564147312636</v>
+      </c>
+      <c r="E94" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F94" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" s="4">
+        <v>3</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D95" s="4">
+        <v>7.7572303235388702</v>
+      </c>
+      <c r="E95" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F95" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="4">
+        <v>3</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D96" s="4">
+        <v>8.4669773400453252</v>
+      </c>
+      <c r="E96" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F96" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="4">
+        <v>3</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D97" s="4">
+        <v>8.1811704267172125</v>
+      </c>
+      <c r="E97" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F97" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="4">
+        <v>3</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D98" s="4">
+        <v>7.5416369739287488</v>
+      </c>
+      <c r="E98" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F98" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="4">
+        <v>3</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D99" s="4">
+        <v>9.0609889351891386</v>
+      </c>
+      <c r="E99" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F99" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" s="4">
+        <v>3</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D100" s="4">
+        <v>7.3826508869736571</v>
+      </c>
+      <c r="E100" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F100" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="4">
+        <v>3</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D101" s="4">
+        <v>7.8110289807065714</v>
+      </c>
+      <c r="E101" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F101" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="4">
+        <v>3</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D102" s="4">
+        <v>8.3151297331282219</v>
+      </c>
+      <c r="E102" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F102" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="4">
+        <v>3</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D103" s="4">
+        <v>8.8420311370004505</v>
+      </c>
+      <c r="E103" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F103" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="4">
+        <v>3</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D104" s="4">
+        <v>8.2667663932358053</v>
+      </c>
+      <c r="E104" s="4">
+        <v>7.36</v>
+      </c>
+      <c r="F104" s="4">
+        <v>9.24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" s="4">
+        <v>3</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D105" s="4">
+        <v>11.472983191428829</v>
+      </c>
+      <c r="E105" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F105" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="4">
+        <v>3</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D106" s="4">
+        <v>11.89604400523633</v>
+      </c>
+      <c r="E106" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F106" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="4">
+        <v>3</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D107" s="4">
+        <v>9.5958021358981824</v>
+      </c>
+      <c r="E107" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F107" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" s="4">
+        <v>3</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D108" s="4">
+        <v>10.930423248782111</v>
+      </c>
+      <c r="E108" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F108" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" s="4">
+        <v>3</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D109" s="4">
+        <v>12.093018977350511</v>
+      </c>
+      <c r="E109" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F109" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" s="4">
+        <v>3</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D110" s="4">
+        <v>10.71190830078554</v>
+      </c>
+      <c r="E110" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F110" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" s="4">
+        <v>3</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D111" s="4">
+        <v>10.023171822368109</v>
+      </c>
+      <c r="E111" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F111" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="4">
+        <v>3</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D112" s="4">
+        <v>11.84713486061678</v>
+      </c>
+      <c r="E112" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F112" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" s="4">
+        <v>3</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D113" s="4">
+        <v>11.50399166275727</v>
+      </c>
+      <c r="E113" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F113" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" s="4">
+        <v>3</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D114" s="4">
+        <v>11.17863707751534</v>
+      </c>
+      <c r="E114" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F114" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" s="4">
+        <v>3</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D115" s="4">
+        <v>10.95096815494383</v>
+      </c>
+      <c r="E115" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F115" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" s="4">
+        <v>3</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D116" s="4">
+        <v>10.296805129542429</v>
+      </c>
+      <c r="E116" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F116" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="4">
+        <v>3</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D117" s="4">
+        <v>9.9518802060478482</v>
+      </c>
+      <c r="E117" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F117" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" s="4">
+        <v>3</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D118" s="4">
+        <v>10.053020128210161</v>
+      </c>
+      <c r="E118" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F118" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" s="4">
+        <v>3</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D119" s="4">
+        <v>11.45809241643544</v>
+      </c>
+      <c r="E119" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F119" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="4">
+        <v>3</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D120" s="4">
+        <v>9.8641432258864086</v>
+      </c>
+      <c r="E120" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F120" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" s="4">
+        <v>3</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D121" s="4">
+        <v>10.2348017331327</v>
+      </c>
+      <c r="E121" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F121" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" s="4">
+        <v>3</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D122" s="4">
+        <v>11.193190352593369</v>
+      </c>
+      <c r="E122" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F122" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" s="4">
+        <v>3</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D123" s="4">
+        <v>10.040799309768049</v>
+      </c>
+      <c r="E123" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F123" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="4">
+        <v>3</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D124" s="4">
+        <v>11.92528030212581</v>
+      </c>
+      <c r="E124" s="4">
+        <v>9.57</v>
+      </c>
+      <c r="F124" s="4">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="4">
+        <v>4</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D125" s="4">
+        <v>16.10776452666158</v>
+      </c>
+      <c r="E125" s="4">
+        <v>14</v>
+      </c>
+      <c r="F125" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="4">
+        <v>4</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D126" s="4">
+        <v>14.10040167170173</v>
+      </c>
+      <c r="E126" s="4">
+        <v>14</v>
+      </c>
+      <c r="F126" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="4">
+        <v>4</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D127" s="4">
+        <v>16.12696580819582</v>
+      </c>
+      <c r="E127" s="4">
+        <v>14</v>
+      </c>
+      <c r="F127" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B128" s="4">
+        <v>4</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D128" s="4">
+        <v>15.943309059039089</v>
+      </c>
+      <c r="E128" s="4">
+        <v>14</v>
+      </c>
+      <c r="F128" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B129" s="4">
+        <v>4</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D129" s="4">
+        <v>14.64647577298614</v>
+      </c>
+      <c r="E129" s="4">
+        <v>14</v>
+      </c>
+      <c r="F129" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B130" s="4">
+        <v>4</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D130" s="4">
+        <v>14.297238046987561</v>
+      </c>
+      <c r="E130" s="4">
+        <v>14</v>
+      </c>
+      <c r="F130" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B131" s="4">
+        <v>4</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D131" s="4">
+        <v>15.08711713028832</v>
+      </c>
+      <c r="E131" s="4">
+        <v>14</v>
+      </c>
+      <c r="F131" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B132" s="4">
+        <v>4</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D132" s="4">
+        <v>15.51493088700061</v>
+      </c>
+      <c r="E132" s="4">
+        <v>14</v>
+      </c>
+      <c r="F132" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B133" s="4">
+        <v>4</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D133" s="4">
+        <v>14.58630944884519</v>
+      </c>
+      <c r="E133" s="4">
+        <v>14</v>
+      </c>
+      <c r="F133" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" s="4">
+        <v>4</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D134" s="4">
+        <v>15.94842008788304</v>
+      </c>
+      <c r="E134" s="4">
+        <v>14</v>
+      </c>
+      <c r="F134" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="4">
+        <v>4</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D135" s="4">
+        <v>15.60240263007845</v>
+      </c>
+      <c r="E135" s="4">
+        <v>14</v>
+      </c>
+      <c r="F135" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136" s="4">
+        <v>4</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D136" s="4">
+        <v>14.520280484187429</v>
+      </c>
+      <c r="E136" s="4">
+        <v>14</v>
+      </c>
+      <c r="F136" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" s="4">
+        <v>4</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D137" s="4">
+        <v>15.68550590542581</v>
+      </c>
+      <c r="E137" s="4">
+        <v>14</v>
+      </c>
+      <c r="F137" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" s="4">
+        <v>4</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D138" s="4">
+        <v>15.769366763121671</v>
+      </c>
+      <c r="E138" s="4">
+        <v>14</v>
+      </c>
+      <c r="F138" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B139" s="4">
+        <v>4</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D139" s="4">
+        <v>14.499501005961401</v>
+      </c>
+      <c r="E139" s="4">
+        <v>14</v>
+      </c>
+      <c r="F139" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B140" s="4">
+        <v>4</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D140" s="4">
+        <v>16.076034870137612</v>
+      </c>
+      <c r="E140" s="4">
+        <v>14</v>
+      </c>
+      <c r="F140" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" s="4">
+        <v>4</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D141" s="4">
+        <v>15.02899034280003</v>
+      </c>
+      <c r="E141" s="4">
+        <v>14</v>
+      </c>
+      <c r="F141" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="4">
+        <v>4</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D142" s="4">
+        <v>15.108859841700349</v>
+      </c>
+      <c r="E142" s="4">
+        <v>14</v>
+      </c>
+      <c r="F142" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" s="4">
+        <v>4</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D143" s="4">
+        <v>15.582954315723221</v>
+      </c>
+      <c r="E143" s="4">
+        <v>14</v>
+      </c>
+      <c r="F143" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144" s="4">
+        <v>4</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D144" s="4">
+        <v>15.550067667426321</v>
+      </c>
+      <c r="E144" s="4">
+        <v>14</v>
+      </c>
+      <c r="F144" s="4">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="4">
+        <v>4</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D145" s="4">
+        <v>12.45179437766379</v>
+      </c>
+      <c r="E145" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F145" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="4">
+        <v>4</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D146" s="4">
+        <v>11.534223093689491</v>
+      </c>
+      <c r="E146" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F146" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B147" s="4">
+        <v>4</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D147" s="4">
+        <v>12.28794651531344</v>
+      </c>
+      <c r="E147" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F147" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" s="4">
+        <v>4</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D148" s="4">
+        <v>14.0957658355108</v>
+      </c>
+      <c r="E148" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F148" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" s="4">
+        <v>4</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D149" s="4">
+        <v>13.69626487321494</v>
+      </c>
+      <c r="E149" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F149" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" s="4">
+        <v>4</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D150" s="4">
+        <v>13.799420826962979</v>
+      </c>
+      <c r="E150" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F150" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" s="4">
+        <v>4</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D151" s="4">
+        <v>14.190034372436889</v>
+      </c>
+      <c r="E151" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F151" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B152" s="4">
+        <v>4</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D152" s="4">
+        <v>13.64588594655234</v>
+      </c>
+      <c r="E152" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F152" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B153" s="4">
+        <v>4</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D153" s="4">
+        <v>11.72767008797725</v>
+      </c>
+      <c r="E153" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F153" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B154" s="4">
+        <v>4</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D154" s="4">
+        <v>12.27105896899541</v>
+      </c>
+      <c r="E154" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F154" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B155" s="4">
+        <v>4</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D155" s="4">
+        <v>12.978206326536929</v>
+      </c>
+      <c r="E155" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F155" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156" s="4">
+        <v>4</v>
+      </c>
+      <c r="C156" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D156" s="4">
+        <v>13.20220997794344</v>
+      </c>
+      <c r="E156" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F156" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B157" s="4">
+        <v>4</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D157" s="4">
+        <v>12.66877511224674</v>
+      </c>
+      <c r="E157" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F157" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158" s="4">
+        <v>4</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D158" s="4">
+        <v>12.13967355821905</v>
+      </c>
+      <c r="E158" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F158" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159" s="4">
+        <v>4</v>
+      </c>
+      <c r="C159" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D159" s="4">
+        <v>12.741678006064481</v>
+      </c>
+      <c r="E159" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F159" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B160" s="4">
+        <v>4</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D160" s="4">
+        <v>12.50469346162507</v>
+      </c>
+      <c r="E160" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F160" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B161" s="4">
+        <v>4</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D161" s="4">
+        <v>14.1224726456166</v>
+      </c>
+      <c r="E161" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F161" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B162" s="4">
+        <v>4</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D162" s="4">
+        <v>11.79244390340499</v>
+      </c>
+      <c r="E162" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F162" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B163" s="4">
+        <v>4</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D163" s="4">
+        <v>12.81755745288593</v>
+      </c>
+      <c r="E163" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F163" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B164" s="4">
+        <v>4</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D164" s="4">
+        <v>12.158180797831729</v>
+      </c>
+      <c r="E164" s="4">
+        <v>11.52</v>
+      </c>
+      <c r="F164" s="4">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" s="4">
+        <v>4</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D165" s="4">
+        <v>17.559703049320611</v>
+      </c>
+      <c r="E165" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F165" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B166" s="4">
+        <v>4</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D166" s="4">
+        <v>19.944097399281659</v>
+      </c>
+      <c r="E166" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F166" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B167" s="4">
+        <v>4</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D167" s="4">
+        <v>20.699577391260689</v>
+      </c>
+      <c r="E167" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F167" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B168" s="4">
+        <v>4</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D168" s="4">
+        <v>18.943053055945381</v>
+      </c>
+      <c r="E168" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F168" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B169" s="4">
+        <v>4</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D169" s="4">
+        <v>18.592755067538789</v>
+      </c>
+      <c r="E169" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F169" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" s="4">
+        <v>4</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D170" s="4">
+        <v>20.55219490694618</v>
+      </c>
+      <c r="E170" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F170" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B171" s="4">
+        <v>4</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D171" s="4">
+        <v>19.497555643858441</v>
+      </c>
+      <c r="E171" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F171" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B172" s="4">
+        <v>4</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D172" s="4">
+        <v>20.209684737924821</v>
+      </c>
+      <c r="E172" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F172" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173" s="4">
+        <v>4</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D173" s="4">
+        <v>18.551859497555359</v>
+      </c>
+      <c r="E173" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F173" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B174" s="4">
+        <v>4</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D174" s="4">
+        <v>21.372539337812739</v>
+      </c>
+      <c r="E174" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F174" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B175" s="4">
+        <v>4</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D175" s="4">
+        <v>18.45416414133274</v>
+      </c>
+      <c r="E175" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F175" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B176" s="4">
+        <v>4</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D176" s="4">
+        <v>21.371078694969881</v>
+      </c>
+      <c r="E176" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F176" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B177" s="4">
+        <v>4</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D177" s="4">
+        <v>20.689949300627781</v>
+      </c>
+      <c r="E177" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F177" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B178" s="4">
+        <v>4</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D178" s="4">
+        <v>19.219231622899368</v>
+      </c>
+      <c r="E178" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F178" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B179" s="4">
+        <v>4</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D179" s="4">
+        <v>20.030005221241399</v>
+      </c>
+      <c r="E179" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F179" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B180" s="4">
+        <v>4</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D180" s="4">
+        <v>21.179531384783189</v>
+      </c>
+      <c r="E180" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F180" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B181" s="4">
+        <v>4</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D181" s="4">
+        <v>17.55489717072091</v>
+      </c>
+      <c r="E181" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F181" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B182" s="4">
+        <v>4</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D182" s="4">
+        <v>19.170842443690479</v>
+      </c>
+      <c r="E182" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F182" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B183" s="4">
+        <v>4</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D183" s="4">
+        <v>16.983760273912569</v>
+      </c>
+      <c r="E183" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F183" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B184" s="4">
+        <v>4</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D184" s="4">
+        <v>20.277912564864749</v>
+      </c>
+      <c r="E184" s="4">
+        <v>16.98</v>
+      </c>
+      <c r="F184" s="4">
+        <v>21.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A488C0B3-771B-314C-9B9D-BB0181F5181B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>